<commit_message>
Update bulk-service according to new excel formats
</commit_message>
<xml_diff>
--- a/bulk-service/src/excelFilesExample/changeRoleHierarchyBulk.xlsx
+++ b/bulk-service/src/excelFilesExample/changeRoleHierarchyBulk.xlsx
@@ -1,34 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stein\Desktop\excelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liron\Desktop\עבודה-energyteam\Lego\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42A3CD0-9FE1-41B9-9BC2-554094FC6243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6095FBA-528B-4DAC-8084-1A4D48387EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C14B5B40-B5B4-4DEB-9023-5BFFA03EBB54}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="פורמט הגשה לבקשת מעבר היררכיה" sheetId="3" r:id="rId1"/>
+    <sheet name="הסבר להגשת הבקשה-לא להגשה!!!" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>יוזר</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>t1@gmail.com</t>
   </si>
@@ -90,39 +97,235 @@
     <t>ליצן 5</t>
   </si>
   <si>
-    <t>ליצן 6</t>
+    <t>יוזר (TXXXXXX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">קוסם בכיר </t>
+  </si>
+  <si>
+    <t>טופס הסבר להגשת בקשת באלק! אין צורך להגיש גליון הסבר זה בבקשה!</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>משתמש LEGO יקר!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+באפשרותך להגיש בקשה מרובה עבור מעבר תפקידים בין היררכיות. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>אנא וודא את הנתונים הבאים טרם הגשת הבקשה:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. שדה "יוזר"- עליך להכניס את מספרי הT אותם תרצה להעביר היררכיה. לדוגמה "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T012345</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 
+2. שדה "שם תפקיד נוכחי"- עליך להכניס את שם התפקיד של אותו הT שרשמת. לדוגמה עבור הT012345 שם התפקיד הוא "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>משק 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>". את שם התפקיד כמובן אפשר למצוא במערכת הLEGO בפרטי התפקיד/ טבלת התפקידים/ תחת ההיררכיה הקיימת אם אינך זוכר במדיוק.
+3. שדה "שם תפקיד חדש (אופציונאלי)"- באפשרותך להכניס שם חדש לתפקיד קיים ולשנות את השם הנוכחי. שדה שאינו חובה למילוי
+עם סיום מילוי טופס פורמט הגשה לבקשת מעבר היררכיה יש לשמור אותו על עמדת העבודה ולהעלות למערכת LEGO להגשת הבקשה.
+אין צורך להשתמש בגיליון זה. ניתן להתעלם ממנו/ ניתן למחוק אותו לפני הגשת הבקשה.
+* יש לוודא תקינות הקובץ טרם הגשתו על מנת למנוע עבודה כפולה עבורך במידה ואחד מהנתונים אינו תקין.</t>
+    </r>
+  </si>
+  <si>
+    <t>טבלה לדוגמה:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -130,18 +333,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="20% - הדגשה1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="היפר-קישור" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -156,20 +409,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73B14437-1D36-4E57-A883-B747847D0C25}" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9" xr:uid="{73B14437-1D36-4E57-A883-B747847D0C25}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{665C1B38-D08B-4477-8266-3A09C65355EC}" name="שם תפקיד חדש (אופציונלי)"/>
-    <tableColumn id="2" xr3:uid="{1BA4EE5E-D55F-46F5-AE70-7F883272A1ED}" name="שם תפקיד נוכחי"/>
-    <tableColumn id="3" xr3:uid="{C41A1F1F-FC49-481F-B798-886FC4805D56}" name="יוזר"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -185,7 +426,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -197,7 +438,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -244,6 +485,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -279,6 +537,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,117 +705,204 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C011A91-29B6-458C-8DA7-210F40FD505E}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778ACC16-8C73-4C08-8F07-19A1FE2BCC9F}">
+  <dimension ref="A2:L15"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" ht="25" x14ac:dyDescent="0.5">
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="196" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{F671F06C-22A6-49FD-A9C3-F4F032814643}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{CD6410AB-9B77-4955-B912-ABDB4845879A}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{23ADB1A1-35B3-4301-97AE-38DA074472D8}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{B3AFDFF7-837C-445A-8EB7-9A04B0BB029D}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{3A6CDB66-2009-4C11-BDF5-6133E42B2D8C}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{A0249B03-6B78-46DB-8966-99081434F974}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{3014C767-6C99-4ABD-A029-5D1FCD30E5B3}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{B0A79E40-E2BD-45BB-A7FB-CB5D191497E6}"/>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{BEBDE697-F89F-4D7B-AB24-A77C27E9325E}"/>
+    <hyperlink ref="A9" r:id="rId2" xr:uid="{E8501A3E-6BF5-4605-94D6-3113AD7E7499}"/>
+    <hyperlink ref="A10" r:id="rId3" xr:uid="{53E58975-2F8A-4D8E-8968-4FFDAF781CAE}"/>
+    <hyperlink ref="A11" r:id="rId4" xr:uid="{31922F09-03AF-44E1-BCD0-FB7E25F27F32}"/>
+    <hyperlink ref="A12" r:id="rId5" xr:uid="{6E37119B-8C82-4116-922F-A2D6AB76D79B}"/>
+    <hyperlink ref="A13" r:id="rId6" xr:uid="{84768B69-1724-459A-B89D-36BA51FEFC70}"/>
+    <hyperlink ref="A14" r:id="rId7" xr:uid="{FDFF9E6D-1E83-44F9-ADDF-F8AC55B62664}"/>
+    <hyperlink ref="A15" r:id="rId8" xr:uid="{8DB60E05-25F0-41C1-A307-A3B8157AF20C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId9"/>
-  </tableParts>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>